<commit_message>
feature: programs choice and sorting added
</commit_message>
<xml_diff>
--- a/input/Programlar.xlsx
+++ b/input/Programlar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>İsim</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>https://www.youthall.com/tr/yenibirlider/lead21-fellowship-programi_7/</t>
+  </si>
+  <si>
+    <t>Koç Ctrl+ Future</t>
+  </si>
+  <si>
+    <t>02.07.2023</t>
+  </si>
+  <si>
+    <t>https://www.kockariyerim.com/jobAds/koc-toplulugu-sirketleri-ctrl-future-programi/0d41fa03-0bc5-4ba3-b272-8f161a71b238</t>
   </si>
 </sst>
 </file>
@@ -57,11 +66,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -89,14 +98,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -109,22 +111,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -134,14 +122,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,7 +144,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,6 +173,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -187,38 +190,44 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,30 +242,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -269,7 +362,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,49 +386,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,49 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,31 +416,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,6 +433,65 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -465,77 +533,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -548,127 +557,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1002,7 +1011,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1064,7 +1073,16 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="4:4">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="4:4">

</xml_diff>

<commit_message>
bug: date bug solved for programs page
</commit_message>
<xml_diff>
--- a/input/Programlar.xlsx
+++ b/input/Programlar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>İsim</t>
   </si>
@@ -59,6 +59,21 @@
   </si>
   <si>
     <t>https://www.kockariyerim.com/jobAds/koc-toplulugu-sirketleri-ctrl-future-programi/0d41fa03-0bc5-4ba3-b272-8f161a71b238</t>
+  </si>
+  <si>
+    <t>Akbank Fellowship</t>
+  </si>
+  <si>
+    <t>https://form.jotform.com/231551887039968</t>
+  </si>
+  <si>
+    <t>Aspire Leaders</t>
+  </si>
+  <si>
+    <t>11.01.2023</t>
+  </si>
+  <si>
+    <t>https://apply.aspireleaders.org/f/64413a183b5d0038f900087e</t>
   </si>
 </sst>
 </file>
@@ -66,11 +81,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -97,6 +112,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -105,7 +128,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,9 +196,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,29 +226,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,75 +242,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,25 +257,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,151 +431,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,8 +454,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -460,6 +475,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -471,17 +495,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -510,15 +523,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -533,151 +537,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1011,7 +1026,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1085,10 +1100,28 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="4:4">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="4:4">
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="4:4">

</xml_diff>